<commit_message>
02 Nov no 4
</commit_message>
<xml_diff>
--- a/01.MODELO PERSEPOLIS/02.Ejecucion/06.Frente Finanzas y Legal/modelo financiacion/modelo financiero.xlsx
+++ b/01.MODELO PERSEPOLIS/02.Ejecucion/06.Frente Finanzas y Legal/modelo financiacion/modelo financiero.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19800" windowHeight="8910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19800" windowHeight="8910" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Presentacion" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Fuentes de Financiacion" sheetId="3" r:id="rId4"/>
     <sheet name="Tablas" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3599,9 +3599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3821,8 +3819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,7 +3915,6 @@
         <v>2</v>
       </c>
       <c r="B6" s="80">
-        <f>+Presentacion!C10</f>
         <v>1</v>
       </c>
       <c r="D6" s="13" t="s">
@@ -4801,7 +4798,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V108"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7895,8 +7894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>